<commit_message>
JAMP - Added CFD extraction capabilities
</commit_message>
<xml_diff>
--- a/logs/20210510/pandas_simple210510a_pivot.xlsx
+++ b/logs/20210510/pandas_simple210510a_pivot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/dev/jamp/logs/20210510/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C855D-135A-1B4D-AA13-95A16C057302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868BEEBD-C49B-A743-9BE2-2724F0825110}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="1120" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
   <si>
     <t>Team</t>
   </si>
@@ -262,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,21 +278,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -309,15 +337,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -328,11 +357,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -767,89 +795,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$4:$A$57</c:f>
+              <c:f>Sheet1!$A$4:$A$31</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="26"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Sprint 1 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Sprint 2 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Sprint 3 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Sprint 4 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Sprint 5 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Sprint 6 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Sprint 7 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Sprint 8 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Sprint 9 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Sprint 10 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Sprint 11 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Sprint 12 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Sprint 13 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Sprint 14 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Sprint 15 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Sprint 16 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Sprint 17 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Sprint 18 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Sprint 19 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Sprint 20 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Sprint 21 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Sprint 22 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Sprint 23 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>Sprint 24 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Sprint 25 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Sprint 26 (IDAP 2021)</c:v>
-                  </c:pt>
-                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>1</c:v>
@@ -940,7 +888,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$57</c:f>
+              <c:f>Sheet1!$B$4:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1133,89 +1081,9 @@
           </c:trendline>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$4:$A$57</c:f>
+              <c:f>Sheet1!$A$4:$A$31</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="26"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Sprint 1 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Sprint 2 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Sprint 3 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Sprint 4 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Sprint 5 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Sprint 6 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Sprint 7 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Sprint 8 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Sprint 9 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Sprint 10 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Sprint 11 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Sprint 12 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Sprint 13 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Sprint 14 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Sprint 15 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Sprint 16 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Sprint 17 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Sprint 18 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Sprint 19 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Sprint 20 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Sprint 21 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Sprint 22 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Sprint 23 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>Sprint 24 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Sprint 25 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Sprint 26 (IDAP 2021)</c:v>
-                  </c:pt>
-                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>1</c:v>
@@ -1306,7 +1174,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$57</c:f>
+              <c:f>Sheet1!$C$4:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1474,89 +1342,9 @@
           </c:trendline>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$4:$A$57</c:f>
+              <c:f>Sheet1!$A$4:$A$31</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="26"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Sprint 1 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Sprint 2 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Sprint 3 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Sprint 4 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Sprint 5 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Sprint 6 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Sprint 7 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Sprint 8 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Sprint 9 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Sprint 10 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Sprint 11 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Sprint 12 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Sprint 13 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Sprint 14 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Sprint 15 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Sprint 16 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Sprint 17 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Sprint 18 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Sprint 19 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>Sprint 20 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Sprint 21 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Sprint 22 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>Sprint 23 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>Sprint 24 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>Sprint 25 (IDAP 2021)</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Sprint 26 (IDAP 2021)</c:v>
-                  </c:pt>
-                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>1</c:v>
@@ -1647,7 +1435,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$57</c:f>
+              <c:f>Sheet1!$D$4:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -2510,7 +2298,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E7980299-DDE0-454F-AB79-66B0DC0D4DC0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="164" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3739,7 +3527,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C295C436-5C3E-7B4E-A581-65F09919460D}" name="PivotTable4" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A3:D57" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:D31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -3820,34 +3608,34 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="28">
-        <item x="1"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item t="default"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item t="default" sd="0"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -3856,165 +3644,87 @@
     <field x="18"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="54">
+  <rowItems count="28">
     <i>
       <x v="1"/>
     </i>
     <i r="1">
       <x v="1"/>
     </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
     <i r="1">
       <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="22"/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
-    <i r="2">
-      <x v="37"/>
-    </i>
     <i r="1">
       <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="38"/>
     </i>
     <i r="1">
       <x v="5"/>
     </i>
-    <i r="2">
-      <x v="40"/>
-    </i>
     <i r="1">
       <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="42"/>
     </i>
     <i r="1">
       <x v="7"/>
     </i>
-    <i r="2">
-      <x v="44"/>
-    </i>
     <i r="1">
       <x v="8"/>
-    </i>
-    <i r="2">
-      <x v="46"/>
     </i>
     <i r="1">
       <x v="9"/>
     </i>
-    <i r="2">
-      <x v="48"/>
-    </i>
     <i r="1">
       <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
     </i>
     <i r="1">
       <x v="11"/>
     </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="12"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
     </i>
     <i r="1">
       <x v="13"/>
     </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
     <i r="1">
       <x v="14"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
     </i>
     <i r="1">
       <x v="15"/>
     </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
     <i r="1">
       <x v="16"/>
     </i>
-    <i r="2">
-      <x v="15"/>
-    </i>
     <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="2">
       <x v="17"/>
     </i>
     <i r="1">
       <x v="18"/>
     </i>
-    <i r="2">
-      <x v="19"/>
-    </i>
     <i r="1">
       <x v="19"/>
-    </i>
-    <i r="2">
-      <x v="21"/>
     </i>
     <i r="1">
       <x v="20"/>
     </i>
-    <i r="2">
-      <x v="24"/>
-    </i>
     <i r="1">
       <x v="21"/>
-    </i>
-    <i r="2">
-      <x v="26"/>
     </i>
     <i r="1">
       <x v="22"/>
     </i>
-    <i r="2">
-      <x v="28"/>
-    </i>
     <i r="1">
       <x v="23"/>
-    </i>
-    <i r="2">
-      <x v="30"/>
     </i>
     <i r="1">
       <x v="24"/>
     </i>
-    <i r="2">
-      <x v="32"/>
-    </i>
     <i r="1">
       <x v="25"/>
     </i>
-    <i r="2">
-      <x v="34"/>
-    </i>
     <i r="1">
       <x v="26"/>
-    </i>
-    <i r="2">
-      <x v="36"/>
     </i>
     <i t="grand">
       <x/>
@@ -4433,22 +4143,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F37FA4E-5455-8C45-AE80-725037EBE8C5}">
-  <dimension ref="A3:D57"/>
+  <dimension ref="A3:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
@@ -4462,7 +4172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>2021</v>
       </c>
@@ -4476,7 +4186,7 @@
         <v>8.6072179010405758</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -4490,595 +4200,299 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>40</v>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6">
+        <v>2</v>
       </c>
       <c r="B6" s="5">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="5">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>1.023255813953488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6">
+        <v>4</v>
       </c>
       <c r="B8" s="5">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C9" s="5">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D9" s="5">
-        <v>1.023255813953488</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>42</v>
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6">
+        <v>6</v>
       </c>
       <c r="B10" s="5">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D10" s="5">
-        <v>1.023255813953488</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>43</v>
+        <v>0.86486486486486491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6">
+        <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.796875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C13" s="5">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D13" s="5">
-        <v>0.97222222222222221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6">
+        <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>72</v>
-      </c>
-      <c r="C14" s="5">
-        <v>70</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.97222222222222221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5">
-        <v>68</v>
-      </c>
-      <c r="C15" s="5">
-        <v>68</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>45</v>
+        <v>21</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="6">
+        <v>12</v>
       </c>
       <c r="B16" s="5">
-        <v>68</v>
-      </c>
-      <c r="C16" s="5">
-        <v>68</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="6">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
-        <v>74</v>
-      </c>
-      <c r="C17" s="5">
-        <v>64</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.86486486486486491</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>46</v>
+        <v>8</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6">
+        <v>14</v>
       </c>
       <c r="B18" s="5">
-        <v>74</v>
-      </c>
-      <c r="C18" s="5">
-        <v>64</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.86486486486486491</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="6">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5">
-        <v>64</v>
-      </c>
-      <c r="C19" s="5">
-        <v>51</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.796875</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>47</v>
+        <v>0</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="6">
+        <v>16</v>
       </c>
       <c r="B20" s="5">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5">
-        <v>51</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.796875</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="6">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5">
-        <v>100</v>
-      </c>
-      <c r="C21" s="5">
-        <v>95</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6">
+        <v>18</v>
       </c>
       <c r="B22" s="5">
-        <v>100</v>
-      </c>
-      <c r="C22" s="5">
-        <v>95</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="6">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>49</v>
+    <row r="24" spans="1:4">
+      <c r="A24" s="6">
+        <v>20</v>
       </c>
       <c r="B24" s="5">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="6">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>50</v>
+    <row r="26" spans="1:4">
+      <c r="A26" s="6">
+        <v>22</v>
       </c>
       <c r="B26" s="5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="6">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>51</v>
+    <row r="28" spans="1:4">
+      <c r="A28" s="6">
+        <v>24</v>
       </c>
       <c r="B28" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="6">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>52</v>
+    <row r="30" spans="1:4">
+      <c r="A30" s="6">
+        <v>26</v>
       </c>
       <c r="B30" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
-        <v>14</v>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B31" s="5">
-        <v>0</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="5">
-        <v>0</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>15</v>
-      </c>
-      <c r="B33" s="5">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
-        <v>16</v>
-      </c>
-      <c r="B35" s="5">
-        <v>0</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="5">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
-        <v>17</v>
-      </c>
-      <c r="B37" s="5">
-        <v>0</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="5">
-        <v>0</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
-        <v>18</v>
-      </c>
-      <c r="B39" s="5">
-        <v>0</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="5">
-        <v>0</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>19</v>
-      </c>
-      <c r="B41" s="5">
-        <v>0</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="5">
-        <v>0</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
-        <v>20</v>
-      </c>
-      <c r="B43" s="5">
-        <v>0</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
-        <v>21</v>
-      </c>
-      <c r="B45" s="5">
-        <v>0</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
-        <v>22</v>
-      </c>
-      <c r="B47" s="5">
-        <v>0</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
-        <v>23</v>
-      </c>
-      <c r="B49" s="5">
-        <v>0</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="5">
-        <v>0</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
-        <v>24</v>
-      </c>
-      <c r="B51" s="5">
-        <v>0</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" s="5">
-        <v>0</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
-        <v>25</v>
-      </c>
-      <c r="B53" s="5">
-        <v>0</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="5">
-        <v>0</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6">
-        <v>26</v>
-      </c>
-      <c r="B55" s="5">
-        <v>0</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="5">
-        <v>0</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="5">
         <v>654</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C31" s="5">
         <v>519</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D31" s="5">
         <v>8.6072179010405758</v>
       </c>
     </row>
@@ -5091,12 +4505,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
@@ -5104,7 +4518,7 @@
     <col min="4" max="17" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="137" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="137">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5163,7 +4577,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5218,7 +4632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5270,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5319,7 +4733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5371,7 +4785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5423,7 +4837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -5475,7 +4889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -5524,7 +4938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5576,7 +4990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5631,7 +5045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -5683,7 +5097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5735,7 +5149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5787,7 +5201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5839,7 +5253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -5891,7 +5305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -5943,7 +5357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5998,7 +5412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -6050,7 +5464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -6099,7 +5513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -6148,7 +5562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -6197,7 +5611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -6246,7 +5660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -6298,7 +5712,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -6347,7 +5761,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -6396,7 +5810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -6445,7 +5859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -6506,7 +5920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -6564,7 +5978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -6622,7 +6036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -6677,7 +6091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -6735,7 +6149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -6796,7 +6210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -6854,7 +6268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -6903,7 +6317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -6949,7 +6363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -6995,7 +6409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -7041,7 +6455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="16">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -7076,12 +6490,12 @@
         <f>IFERROR(VALUE(LEFT(RIGHT(Table1[[#This Row],[Sprint]],5),4)),2020)</f>
         <v>2021</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="7">
         <f>IFERROR(VALUE(MID(Table1[[#This Row],[Sprint]],LEN("Sprint "),3)),12)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -7121,7 +6535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -7161,7 +6575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -7201,7 +6615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -7241,7 +6655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -7281,7 +6695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -7321,7 +6735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -7361,7 +6775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -7401,7 +6815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -7441,7 +6855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -7481,7 +6895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -7521,7 +6935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>16</v>
       </c>

</xml_diff>